<commit_message>
14 april 2022 10pm
</commit_message>
<xml_diff>
--- a/TestBits Assessment-open/data tambahan/data driven.xlsx
+++ b/TestBits Assessment-open/data tambahan/data driven.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syazw\Documents\GitHub\NewSyazwan_KatalonWebTesting_AssessmentProject\TestBits Assessment-open\data tambahan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE99E72B-E0AA-4040-B92E-C20F92245E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0927FA-C8AC-4290-8CFA-7437CE37ED09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="1185" windowWidth="13635" windowHeight="9345" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="candidate" sheetId="1" r:id="rId1"/>
     <sheet name="location" sheetId="2" r:id="rId2"/>
     <sheet name="member" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="vacancies" sheetId="4" r:id="rId4"/>
+    <sheet name="Employee" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Fname</t>
   </si>
@@ -88,6 +89,36 @@
   </si>
   <si>
     <t>Apps Developer</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Middle name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Abu</t>
+  </si>
+  <si>
+    <t>Mohd</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>abumadkhan</t>
+  </si>
+  <si>
+    <t>Ahmad</t>
+  </si>
+  <si>
+    <t>ahmadkhan</t>
   </si>
 </sst>
 </file>
@@ -418,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -563,4 +594,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC87EF6-F17A-4BC5-8BD9-DE5F0034B2B9}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>